<commit_message>
added test for loading named tables from excel
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -18,42 +18,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>mgrahovac</author>
-  </authors>
-  <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>mgrahovac:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value ensures that each run with identical inputs produces identical outputs</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>a</t>
   </si>
@@ -89,12 +55,6 @@
   </si>
   <si>
     <t>cc</t>
-  </si>
-  <si>
-    <t>Sample Size</t>
-  </si>
-  <si>
-    <t>Seed Value</t>
   </si>
   <si>
     <t>Output Path</t>
@@ -113,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,19 +207,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -689,13 +636,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="run_parameters" displayName="run_parameters" ref="B2:E3" totalsRowShown="0">
-  <autoFilter ref="B2:E3"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Sample Size"/>
-    <tableColumn id="2" name="Seed Value"/>
-    <tableColumn id="3" name="Output Path"/>
-    <tableColumn id="4" name="Version"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Output Path"/>
+    <tableColumn id="2" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -963,11 +908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,12 +924,6 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="J2" t="s">
         <v>3</v>
       </c>
@@ -996,17 +935,11 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>165798</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1086,11 +1019,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="3">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started refactoring for #3
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -9,17 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22152"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22155"/>
   </bookViews>
   <sheets>
-    <sheet name="test - Copy" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="xlsx_named_range1">test!$J$16:$K$18</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>a</t>
   </si>
@@ -67,6 +70,21 @@
   </si>
   <si>
     <t>vTest</t>
+  </si>
+  <si>
+    <t>nam_ran_col1</t>
+  </si>
+  <si>
+    <t>val1</t>
+  </si>
+  <si>
+    <t>val2</t>
+  </si>
+  <si>
+    <t>val3</t>
+  </si>
+  <si>
+    <t>val4</t>
   </si>
 </sst>
 </file>
@@ -909,15 +927,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L12"/>
+  <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -934,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
@@ -951,7 +969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J4">
         <v>1</v>
       </c>
@@ -962,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>1</v>
       </c>
@@ -973,7 +991,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>6</v>
       </c>
@@ -984,7 +1002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>11</v>
       </c>
@@ -995,7 +1013,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>11</v>
       </c>
@@ -1006,7 +1024,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>11</v>
       </c>
@@ -1015,6 +1033,30 @@
       </c>
       <c r="L12">
         <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added single column table in the test file
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>a</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>col1</t>
+  </si>
+  <si>
+    <t>colA</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -668,6 +674,16 @@
     <tableColumn id="2" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
+  <autoFilter ref="L21:L25"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="colA"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -937,7 +953,7 @@
   <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1050,7 +1066,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J17" t="s">
         <v>17</v>
       </c>
@@ -1058,7 +1074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J18" t="s">
         <v>18</v>
       </c>
@@ -1066,37 +1082,53 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="10:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="10:11" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="10:11" x14ac:dyDescent="0.35">
+      <c r="L22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="10:11" x14ac:dyDescent="0.35">
+      <c r="L23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.35">
+      <c r="L24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J25">
         <v>4</v>
       </c>
+      <c r="L25" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated version to remove ., \, /
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -70,9 +70,6 @@
     <t>output</t>
   </si>
   <si>
-    <t>vTest</t>
-  </si>
-  <si>
     <t>nam_ran_col1</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>v\Test/1.23</t>
   </si>
 </sst>
 </file>
@@ -952,11 +952,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -980,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1060,34 +1063,34 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" t="s">
         <v>22</v>
-      </c>
-      <c r="L21" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.35">
@@ -1119,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="L25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated unit tests, formatted w black, updated version in the setup file to 0.1.1
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\akshaysharma\repos\adapter\adapter\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mg\code\repos\adapter\adapter\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C5FDE2-9290-43E6-8AC0-1433F9BBA983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -88,9 +89,6 @@
     <t>nam_ran_col2</t>
   </si>
   <si>
-    <t>col1</t>
-  </si>
-  <si>
     <t>colA</t>
   </si>
   <si>
@@ -98,12 +96,15 @@
   </si>
   <si>
     <t>v\Test/1.23</t>
+  </si>
+  <si>
+    <t>nam_ran_col11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,45 +644,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="xlsx_table1" displayName="xlsx_table1" ref="J2:L5" totalsRowShown="0">
-  <autoFilter ref="J2:L5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="xlsx_table1" displayName="xlsx_table1" ref="J2:L5" totalsRowShown="0">
+  <autoFilter ref="J2:L5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col_1"/>
-    <tableColumn id="2" name="col_2"/>
-    <tableColumn id="3" name="col_3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="col_1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="col_2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="col_3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="xlsx_table2" displayName="xlsx_table2" ref="J9:L12" totalsRowShown="0">
-  <autoFilter ref="J9:L12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="xlsx_table2" displayName="xlsx_table2" ref="J9:L12" totalsRowShown="0">
+  <autoFilter ref="J9:L12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col_11"/>
-    <tableColumn id="2" name="col_22"/>
-    <tableColumn id="3" name="col_33"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="col_11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="col_22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="col_33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
-  <autoFilter ref="B2:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Output Path"/>
-    <tableColumn id="2" name="Version"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Output Path"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
-  <autoFilter ref="L21:L25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
+  <autoFilter ref="L21:L25" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="colA"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="colA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -949,19 +950,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="AG20" sqref="AG20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -978,12 +979,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -995,7 +996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J4">
         <v>1</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>1</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>11</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>11</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>11</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>15</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1085,15 +1086,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
         <v>21</v>
       </c>
-      <c r="L21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J22">
         <v>1</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J23">
         <v>2</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J24">
         <v>3</v>
       </c>
@@ -1117,12 +1118,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J25">
         <v>4</v>
       </c>
       <c r="L25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed named ranges containing _FilterDatabase in their names, added functionality to read in single value named ranges, removed functionality to convert single value dataframe to the value itself since it throws error when applying column lables
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mg\code\repos\adapter\adapter\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akshaysharma\repos\adapter\adapter\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C5FDE2-9290-43E6-8AC0-1433F9BBA983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23400"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -18,13 +17,14 @@
   <definedNames>
     <definedName name="xlsx_named_range1">test!$J$16:$K$18</definedName>
     <definedName name="xlsx_single_col_range">test!$J$21:$J$25</definedName>
+    <definedName name="xlsx_single_value_named_range">test!$J$29</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>a</t>
   </si>
@@ -99,12 +99,15 @@
   </si>
   <si>
     <t>nam_ran_col11</t>
+  </si>
+  <si>
+    <t>single_value_named_range</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -644,45 +647,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="xlsx_table1" displayName="xlsx_table1" ref="J2:L5" totalsRowShown="0">
-  <autoFilter ref="J2:L5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="xlsx_table1" displayName="xlsx_table1" ref="J2:L5" totalsRowShown="0">
+  <autoFilter ref="J2:L5"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="col_1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="col_2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="col_3"/>
+    <tableColumn id="1" name="col_1"/>
+    <tableColumn id="2" name="col_2"/>
+    <tableColumn id="3" name="col_3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="xlsx_table2" displayName="xlsx_table2" ref="J9:L12" totalsRowShown="0">
-  <autoFilter ref="J9:L12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="xlsx_table2" displayName="xlsx_table2" ref="J9:L12" totalsRowShown="0">
+  <autoFilter ref="J9:L12"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="col_11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="col_22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="col_33"/>
+    <tableColumn id="1" name="col_11"/>
+    <tableColumn id="2" name="col_22"/>
+    <tableColumn id="3" name="col_33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
-  <autoFilter ref="B2:C3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Output Path"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Version"/>
+    <tableColumn id="1" name="Output Path"/>
+    <tableColumn id="2" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
-  <autoFilter ref="L21:L25" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
+  <autoFilter ref="L21:L25"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="colA"/>
+    <tableColumn id="1" name="colA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -950,19 +953,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG20" sqref="AG20"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -979,7 +982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
@@ -996,7 +999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J4">
         <v>1</v>
       </c>
@@ -1007,7 +1010,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J5">
         <v>1</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J9" t="s">
         <v>6</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J10">
         <v>11</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J11">
         <v>11</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J12">
         <v>11</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J16" t="s">
         <v>15</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J17" t="s">
         <v>16</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J21" t="s">
         <v>24</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>1</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J23">
         <v>2</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J24">
         <v>3</v>
       </c>
@@ -1118,12 +1121,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J25">
         <v>4</v>
       </c>
       <c r="L25" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="10:12" x14ac:dyDescent="0.35">
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="10:12" x14ac:dyDescent="0.35">
+      <c r="J29">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on a practical way to write out
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akshaysharma\repos\adapter\adapter\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mg\code\repos\adapter\adapter\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,13 +95,13 @@
     <t>d</t>
   </si>
   <si>
-    <t>v\Test/1.23</t>
-  </si>
-  <si>
     <t>nam_ran_col11</t>
   </si>
   <si>
     <t>single_value_named_range</t>
+  </si>
+  <si>
+    <t>shipper_tests</t>
   </si>
 </sst>
 </file>
@@ -957,15 +957,16 @@
   <dimension ref="B2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -982,12 +983,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -999,7 +1000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J4">
         <v>1</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J5">
         <v>1</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>11</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>11</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>11</v>
       </c>
@@ -1065,7 +1066,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>15</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>16</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1089,15 +1090,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J22">
         <v>1</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J23">
         <v>2</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J24">
         <v>3</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J25">
         <v>4</v>
       </c>
@@ -1129,12 +1130,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="10:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="10:12" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
       <c r="J29">
         <v>123</v>
       </c>

</xml_diff>

<commit_message>
builds and destroys a db based on data connection
</commit_message>
<xml_diff>
--- a/adapter/tests/test.xlsx
+++ b/adapter/tests/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mg\code\repos\adapter\adapter\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792BDEB7-E234-4552-B7B2-7563909D0B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23400"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="23040" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="xlsx_single_col_range">test!$J$21:$J$25</definedName>
     <definedName name="xlsx_single_value_named_range">test!$J$29</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -101,13 +102,13 @@
     <t>single_value_named_range</t>
   </si>
   <si>
-    <t>shipper_tests</t>
+    <t>v123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -647,45 +648,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="xlsx_table1" displayName="xlsx_table1" ref="J2:L5" totalsRowShown="0">
-  <autoFilter ref="J2:L5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="xlsx_table1" displayName="xlsx_table1" ref="J2:L5" totalsRowShown="0">
+  <autoFilter ref="J2:L5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col_1"/>
-    <tableColumn id="2" name="col_2"/>
-    <tableColumn id="3" name="col_3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="col_1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="col_2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="col_3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="xlsx_table2" displayName="xlsx_table2" ref="J9:L12" totalsRowShown="0">
-  <autoFilter ref="J9:L12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="xlsx_table2" displayName="xlsx_table2" ref="J9:L12" totalsRowShown="0">
+  <autoFilter ref="J9:L12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col_11"/>
-    <tableColumn id="2" name="col_22"/>
-    <tableColumn id="3" name="col_33"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="col_11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="col_22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="col_33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
-  <autoFilter ref="B2:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="run_parameters" displayName="run_parameters" ref="B2:C3" totalsRowShown="0">
+  <autoFilter ref="B2:C3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Output Path"/>
-    <tableColumn id="2" name="Version"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Output Path"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
-  <autoFilter ref="L21:L25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="xlsx_single_col_table" displayName="xlsx_single_col_table" ref="L21:L25" totalsRowShown="0">
+  <autoFilter ref="L21:L25" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="colA"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="colA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -953,11 +954,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>